<commit_message>
refactored + multisheet+ optional overwrite
</commit_message>
<xml_diff>
--- a/Gojo Converter/Square_Bulk_Upload_Template.xlsx
+++ b/Gojo Converter/Square_Bulk_Upload_Template.xlsx
@@ -4234,11 +4234,6 @@
           <t>SOFT DRINK CANS</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Souvlaki</t>
-        </is>
-      </c>
       <c r="O10" t="n">
         <v>0.375</v>
       </c>
@@ -4257,11 +4252,6 @@
           <t>WATER</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Souvlaki</t>
-        </is>
-      </c>
       <c r="O11" t="n">
         <v>0.5</v>
       </c>
@@ -4280,13 +4270,8 @@
           <t>ADD SALAMI</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Souvlaki</t>
-        </is>
-      </c>
       <c r="O12" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="T12" t="n">
         <v>3</v>
@@ -4303,13 +4288,8 @@
           <t>ADD HAM</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Souvlaki</t>
-        </is>
-      </c>
       <c r="O13" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="T13" t="n">
         <v>3</v>
@@ -4326,14 +4306,6 @@
           <t>LOW GLUTEN BASE</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Chips</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>0.35</v>
-      </c>
       <c r="T14" t="n">
         <v>5</v>
       </c>
@@ -4349,14 +4321,6 @@
           <t>ADD VEGAN CHEESE</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Snack Pack</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>0.35</v>
-      </c>
       <c r="T15" t="n">
         <v>1.5</v>
       </c>
@@ -4364,279 +4328,405 @@
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>Lamb Souvlaki</t>
+          <t>ICED COFFEE</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Lamb Souvlaki</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Wrap</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>0.18</v>
+          <t>Italian iced coffee- Italian espresso, ice cream, ice, choice of milk</t>
+        </is>
       </c>
       <c r="T16" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chicken Souvlaki</t>
+          <t>OJ</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Chicken Souvlaki</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Chips</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>0.4</v>
+          <t>FRESH ORANGE JUICE</t>
+        </is>
       </c>
       <c r="T17" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mix Souvlaki</t>
+          <t>HAM PIADINA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Mix Souvlaki</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Snack Pack</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>0.3</v>
+          <t>Ham Piadina- Italian tomato salsa, shaved ham, mozzarella, basil</t>
+        </is>
       </c>
       <c r="T18" t="n">
-        <v>21</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>Falafel Souvlaki</t>
+          <t>MUSH PIADINA</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Falafel Souvlaki</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Snack Pack</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>0.05</v>
+          <t>Mushroom piadina- Italian tomato salsa, roast mushroom, mozzar</t>
+        </is>
       </c>
       <c r="T19" t="n">
-        <v>19</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>Chips</t>
+          <t>VEGAN PIADINA</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Chips</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Snack Pack</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>0.45</v>
+          <t>Vegan Piadina- Italian salsa, roast mushroom, vegan cheeese</t>
+        </is>
       </c>
       <c r="T20" t="n">
-        <v>8</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>HSP</t>
+          <t>Ohh la laa</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>HSP- Mix</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Snack Pack</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>0.45</v>
+          <t>Nutella piadina- lashings of Nutella, fresh strawberry</t>
+        </is>
       </c>
       <c r="T21" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t>Breaky Wrap</t>
+          <t>Lamb Souvlaki</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Breakfast Wrap Souvlaki with Hashbrown</t>
+          <t>Lamb Souvlaki</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Souvlaki</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="T22" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" t="inlineStr">
         <is>
-          <t>HashBrown</t>
+          <t>Chicken Souvlaki</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Hashbrown</t>
+          <t>Chicken Souvlaki</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Souvlaki</t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="T23" t="n">
-        <v>2.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t>Lamb Combo</t>
+          <t>Mix Souvlaki</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Lamb Combo</t>
-        </is>
+          <t>Mix Souvlaki</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Souvlaki</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>0.35</v>
       </c>
       <c r="T24" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chicken Combo</t>
+          <t>Falafel Souvlaki</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Chicken Combo</t>
+          <t>Falafel Souvlaki</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Souvlaki</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="T25" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t>Mix Combo</t>
+          <t>Chips</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Mix Combo</t>
+          <t>Chips</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Chips</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="T26" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="C27" t="inlineStr">
         <is>
-          <t>Veg Combo</t>
+          <t>HSP</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Veg Combo</t>
-        </is>
+          <t>HSP- Mix</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Snack Pack</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>0.4</v>
       </c>
       <c r="T27" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="28"/>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Breaky Wrap</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Breakfast Wrap Souvlaki with Hashbrown</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Wrap</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T28" t="n">
+        <v>17</v>
+      </c>
+    </row>
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t>Side of Chips</t>
+          <t>HashBrown</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Side of Chips</t>
-        </is>
+          <t>Hashbrown</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Chips</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>0.05</v>
       </c>
       <c r="T29" t="n">
-        <v>6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="30">
       <c r="C30" t="inlineStr">
         <is>
+          <t>Lamb Combo</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Lamb Combo</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Snack Pack</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="T30" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Chicken Combo</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Chicken Combo</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Snack Pack</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="T31" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Mix Combo</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Mix Combo</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Snack Pack</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="T32" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Veg Combo</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Veg Combo</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Snack Pack</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="T33" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Side of Chips</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Side of Chips</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="inlineStr">
+        <is>
           <t>Cans</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>Cans</t>
         </is>
       </c>
-      <c r="T30" t="n">
+      <c r="O35" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="T35" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" paperSize="0" scale="0" useFirstPageNumber="1" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
accidentally deleted call to conver_weight
</commit_message>
<xml_diff>
--- a/Gojo Converter/Square_Bulk_Upload_Template.xlsx
+++ b/Gojo Converter/Square_Bulk_Upload_Template.xlsx
@@ -4089,10 +4089,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>230g</t>
-        </is>
+      <c r="O3" t="n">
+        <v>0.23</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -4684,10 +4682,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>275g</t>
-        </is>
+      <c r="O4" t="n">
+        <v>0.275</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -5279,10 +5275,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>290g</t>
-        </is>
+      <c r="O5" t="n">
+        <v>0.29</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -5874,10 +5868,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>340g</t>
-        </is>
+      <c r="O6" t="n">
+        <v>0.34</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -6469,10 +6461,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>310g</t>
-        </is>
+      <c r="O7" t="n">
+        <v>0.31</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -7064,10 +7054,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>290g</t>
-        </is>
+      <c r="O8" t="n">
+        <v>0.29</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -7659,10 +7647,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>235g</t>
-        </is>
+      <c r="O9" t="n">
+        <v>0.235</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -8249,10 +8235,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>375ml</t>
-        </is>
+      <c r="O10" t="n">
+        <v>0.375</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -8839,10 +8823,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>500ml</t>
-        </is>
+      <c r="O11" t="n">
+        <v>0.5</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -11769,10 +11751,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>400ML</t>
-        </is>
+      <c r="O16" t="n">
+        <v>0.4</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -12364,10 +12344,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>400ML</t>
-        </is>
+      <c r="O17" t="n">
+        <v>0.4</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -15304,10 +15282,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>350g</t>
-        </is>
+      <c r="O22" t="n">
+        <v>0.35</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -15894,10 +15870,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>350g</t>
-        </is>
+      <c r="O23" t="n">
+        <v>0.35</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -16484,10 +16458,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>350g</t>
-        </is>
+      <c r="O24" t="n">
+        <v>0.35</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -17074,10 +17046,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>350g</t>
-        </is>
+      <c r="O25" t="n">
+        <v>0.35</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -17664,10 +17634,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>180g</t>
-        </is>
+      <c r="O26" t="n">
+        <v>0.18</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -18254,10 +18222,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>400g</t>
-        </is>
+      <c r="O27" t="n">
+        <v>0.4</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -18844,10 +18810,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>300g</t>
-        </is>
+      <c r="O28" t="n">
+        <v>0.3</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -19434,10 +19398,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>50g</t>
-        </is>
+      <c r="O29" t="n">
+        <v>0.05</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -20024,10 +19986,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>450g</t>
-        </is>
+      <c r="O30" t="n">
+        <v>0.45</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -20614,10 +20574,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>450g</t>
-        </is>
+      <c r="O31" t="n">
+        <v>0.45</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
@@ -21204,10 +21162,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>450g</t>
-        </is>
+      <c r="O32" t="n">
+        <v>0.45</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -21794,10 +21750,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>450g</t>
-        </is>
+      <c r="O33" t="n">
+        <v>0.45</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -22379,10 +22333,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>150g</t>
-        </is>
+      <c r="O34" t="n">
+        <v>0.15</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -22969,10 +22921,8 @@
           <t>Prepared food and beverage</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>360g</t>
-        </is>
+      <c r="O35" t="n">
+        <v>0.36</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>

</xml_diff>